<commit_message>
table: Talents change No variable to Str
</commit_message>
<xml_diff>
--- a/FC_tables/Talents.xlsx
+++ b/FC_tables/Talents.xlsx
@@ -1,14 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F878CC9-82BF-4EA0-A45A-B001C51510B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$45</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
@@ -622,7 +626,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -747,6 +751,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -782,6 +803,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -957,12 +995,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +1008,7 @@
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
@@ -1030,7 +1069,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2675,7 +2714,7 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2957,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C43">
         <v>0</v>

</xml_diff>